<commit_message>
function to fit models added, pipeline largely ready, just to add ref SDs for SESOI/ROPE
</commit_message>
<xml_diff>
--- a/protein_meta_data_extraction_sheets.xlsx
+++ b/protein_meta_data_extraction_sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Dropbox\Research\Kieser Australia\Protein\Protein meta\protein_dose_response_meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD05934-6DB8-4B43-8165-F1BA0B1DEB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFC5464-7CFF-4342-BDE0-CE22F752B352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D075C355-E8EB-4DA5-ABDA-21325414D219}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{D075C355-E8EB-4DA5-ABDA-21325414D219}"/>
   </bookViews>
   <sheets>
     <sheet name="Study characteristics" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>PMID</t>
   </si>
@@ -135,6 +133,9 @@
   </si>
   <si>
     <t xml:space="preserve">Proportion Male </t>
+  </si>
+  <si>
+    <t>Sample Size at Timepoint</t>
   </si>
 </sst>
 </file>
@@ -555,13 +556,13 @@
       <selection activeCell="C38" sqref="C38:C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="9" width="28.140625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="9" width="28.1796875" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -599,23 +600,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7602ECBB-AB27-4E81-92AF-26ADC453891B}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="29.28515625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="34.7109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="27.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="31.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" style="2" customWidth="1"/>
+    <col min="1" max="2" width="9.1796875" style="2"/>
+    <col min="3" max="3" width="29.26953125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="34.7265625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="27.26953125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.81640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="31.26953125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="43.7265625" style="2" customWidth="1"/>
     <col min="11" max="11" width="45" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -657,26 +658,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9E3D4C-D5E2-4A46-BB28-F0BDADB22363}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="31.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" style="2"/>
+    <col min="3" max="3" width="31.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="40.1796875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20.7265625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21.90625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -696,12 +698,15 @@
         <v>21</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -714,24 +719,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D2FB40-55E6-40B8-BE4B-7CE947A99C6A}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="39.81640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="35" style="4" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="4"/>
+    <col min="5" max="5" width="25.1796875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" style="4"/>
     <col min="7" max="7" width="23" style="4" customWidth="1"/>
-    <col min="8" max="14" width="21.42578125" style="4"/>
-    <col min="15" max="16384" width="21.42578125" style="1"/>
+    <col min="8" max="14" width="21.453125" style="4"/>
+    <col min="15" max="16384" width="21.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>

</xml_diff>